<commit_message>
Final versi chatbot Radio Untar siap untuk Railway dan WPBot
</commit_message>
<xml_diff>
--- a/dataset_radio_untar.xlsx
+++ b/dataset_radio_untar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gian pratista\OneDrive\Dokumen\chatbot_radio_untar_fix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385046BF-0122-4E6F-A6C0-FBA16D10958E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEEB66E-2B84-457C-9DA0-2EC507FF42B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="226">
   <si>
     <t>Pertanyaan</t>
   </si>
@@ -58,18 +58,12 @@
     <t>Bagaimana cara menjadi penyiar di Radio Untar?</t>
   </si>
   <si>
-    <t>Siapa penyiar yang membawakan program 'Top 10 Chart'?</t>
-  </si>
-  <si>
     <t>Apakah penyiar di Radio Untar hanya dari mahasiswa?</t>
   </si>
   <si>
     <t>Bagaimana cara menghubungi penyiar saat siaran?</t>
   </si>
   <si>
-    <t>Bagaimana cara request lagu di Radio Untar?</t>
-  </si>
-  <si>
     <t>Berapa lama waktu tunggu untuk request lagu?</t>
   </si>
   <si>
@@ -106,21 +100,9 @@
     <t>Anda dapat mendaftar melalui website atau menghubungi penyiar saat siaran berlangsung.</t>
   </si>
   <si>
-    <t>Penyiar tetap di Radio Untar meliputi mahasiswa yang terpilih dalam seleksi tahunan.</t>
-  </si>
-  <si>
     <t>Untuk menjadi penyiar, Anda harus mengikuti seleksi yang dibuka setiap awal semester.</t>
   </si>
   <si>
-    <t>Program 'Top 10 Chart' dibawakan oleh penyiar utama setiap Jumat sore.</t>
-  </si>
-  <si>
-    <t>Mayoritas penyiar adalah mahasiswa, tetapi beberapa dosen dan alumni juga berpartisipasi.</t>
-  </si>
-  <si>
-    <t>Anda dapat menghubungi penyiar melalui media sosial Radio Untar atau fitur chat di website.</t>
-  </si>
-  <si>
     <t>Anda dapat request lagu melalui chatbot atau WhatsApp resmi Radio Untar.</t>
   </si>
   <si>
@@ -304,18 +286,6 @@
     <t>Beberapa program unggulan di Radio Untar antara lain '10 rock action', 'Top 30 ', '20 teratas',dan 'asia in pop'.</t>
   </si>
   <si>
-    <t>Ya, terdapat pogram radio untar night siaran malam dari pukul 18:00 hingga 20:00 WIB yang berisi musik santai dan diskusi ringan.</t>
-  </si>
-  <si>
-    <t>Ya, terdapat program 'campus life' yang ditujukan bagi mahasiswa baru untuk mengenal lingkungan kampus.</t>
-  </si>
-  <si>
-    <t>Kapan program 'spasoda' ditayangkan?</t>
-  </si>
-  <si>
-    <t>Program 'spasoda' ditayangkan setiap Senin sampai jumat dari pukul 10:00 sampai dengan 12:00 WIB.</t>
-  </si>
-  <si>
     <t>Apakah ada program bahasa inggris di Radio Untar?</t>
   </si>
   <si>
@@ -325,9 +295,6 @@
     <t>apa itu segmen spasoda</t>
   </si>
   <si>
-    <t xml:space="preserve">spasoda merupakan singkatan dari 'selamat pagi sobat muda' yang di mulai dari pukul 10:00 sampai dengan 12:00 WIB .membahas seputar ramalan cuaca har ini dan seputar traffic aupdate sekitar Jakarta </t>
-  </si>
-  <si>
     <t>apa itu segmen mn tips&amp; gossip</t>
   </si>
   <si>
@@ -412,18 +379,6 @@
     <t>apa itu segmen obsesi</t>
   </si>
   <si>
-    <t>Merupakan segmen yang membahas seputar tips ataupun gosip yang sedang terjadi, dimulai pada pukul 01.00 sampai dengan pukul 02.00 siang setiap hari senin sampai dengan Jumat</t>
-  </si>
-  <si>
-    <t>Merupakan segmen yang membahas seputar olahraga dimulai pada pukul 02.00 siang sampai dengan pukul 03.00 sore setiap hari Senin</t>
-  </si>
-  <si>
-    <t>Merupakan segmen chart radio Antar dimulai pada pukul 03.00 Sampai dengan pukul 04.00 setiap hari Senin</t>
-  </si>
-  <si>
-    <t>Merupakan segmen yang membahas seputar percintaan tips percintaan dimulai pada pukul 04.00 sore sampai dengan pukul .00 sore</t>
-  </si>
-  <si>
     <t>Merupakan segmen yang membahas hal-hal random ini mulai pukul 6 sore sampai dengan pukul 08.00 malam</t>
   </si>
   <si>
@@ -701,6 +656,48 @@
   </si>
   <si>
     <t>Apakah ada kemungkinan radio 4 di masa depan akan menjadi Fm</t>
+  </si>
+  <si>
+    <t>Ya, terdapat pogram radio untar night, siaran dimulai  dari pukul 18:00 hingga 20:00 WIB yang berisi musik santai dan pembahasan ringan yang berbeda beda di setiap harinya.</t>
+  </si>
+  <si>
+    <t>Ya, terdapat program 'campus life' yang ditujukan bagi mahasiswa baru untuk mengenal lingkungan kampus dan juga informasi sekitar universitas tarumanagara.</t>
+  </si>
+  <si>
+    <t>Kapan program spasoda ditayangkan?</t>
+  </si>
+  <si>
+    <t>Program spasoda ditayangkan setiap hari Senin sampai jumat dari pukul 10:00 sampai dengan 12:00 WIB.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">penyiar rado untar berasal dari mahasiswa universitas tarumanagara yang  sudah mengikuti kegiatan calon crew aktif di radio untar dan sudah melewati beberapa fase penyeleksian penyiar. </t>
+  </si>
+  <si>
+    <t>Siapa penyiar yang membawakan program 10 rockaction?</t>
+  </si>
+  <si>
+    <t>penyiar 10 rock action sekrang adalah acin.</t>
+  </si>
+  <si>
+    <t>benar,penyiar radio untar hanya dari mahasiswa universitas tarumanagara.</t>
+  </si>
+  <si>
+    <t>Bagaimana carameminta putar lagu di Radio Untar?</t>
+  </si>
+  <si>
+    <t>mn tips &amp; gossip segmen yang membahas seputar tips ataupun gosip yang sedang terjadi, dimulai pada pukul 13.00  sampai dengan pukul 14.00 WIB setiap hari senin sampai dengan Jumat</t>
+  </si>
+  <si>
+    <t>RUSH segmen yang membahas seputar olahraga dimulai pada pukul 14.00  sampai dengan pukul 15.00 WIB setiap hari Senin</t>
+  </si>
+  <si>
+    <t>spasoda merupakan singkatan dari 'selamat pagi sobat muda' yang di mulai dari pukul 10:00 sampai dengan 12:00 WIB, membahas seputar ramalan cuaca harI ini dan seputar traffic update sekitar Jakarta.</t>
+  </si>
+  <si>
+    <t>merupakan salah satu segmen chart di radio untar yang dimulai pada pukul 15.00 Sampai dengan pukul 16.00 WIB di setiap hari Senin</t>
+  </si>
+  <si>
+    <t>segmen yang membahas yang membahas seputar percintaan tips percintaan dimulai pada pukul 04.00 sore sampai dengan pukul .00 sore</t>
   </si>
 </sst>
 </file>
@@ -1070,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1093,7 +1090,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1101,7 +1098,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1109,7 +1106,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1117,7 +1114,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1125,7 +1122,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1133,7 +1130,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1141,23 +1138,23 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>214</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1165,7 +1162,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -1173,7 +1170,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -1181,839 +1178,837 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>217</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>220</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B28" t="s">
-        <v>130</v>
+        <v>221</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B29" t="s">
-        <v>131</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
-        <v>132</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B31" t="s">
-        <v>133</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B32" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B33" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B34" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B35" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B37" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B38" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B39" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B40" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B41" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B42" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B43" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B44" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B45" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B46" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B47" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B48" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B49" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B50" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B51" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B52" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B53" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B54" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B55" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="B56" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="B57" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B58" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="B60" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="B61" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="B62" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="B63" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="B64" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="B65" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="B66" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="B67" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="B68" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="B69" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="B70" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="B71" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="B72" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="B73" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="B74" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="B75" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="B76" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="B77" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="B78" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="B79" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="B80" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="B81" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="B82" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="B83" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="B84" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="B85" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="B86" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B87" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="B88" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="B89" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="B90" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="B91" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="B92" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="B93" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="B94" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="B95" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="B96" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="B97" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="B98" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B99" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="B100" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="B101" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="B102" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="B103" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="B104" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="B105" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="B106" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>